<commit_message>
Updated data load with more info
</commit_message>
<xml_diff>
--- a/raw data/DataLoad.xlsx
+++ b/raw data/DataLoad.xlsx
@@ -1,25 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14128"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joe\GovHack2013\SydneyLexicographer\raw data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bvpd\Documents\GitHub\SydneyLexicographer\raw data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19350" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8595"/>
   </bookViews>
   <sheets>
     <sheet name="Output" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Output!$A$1:$G$33</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
   <si>
     <t>http://dos.heuristscholar.org/heurist/php/fetch_file.php/cosLib_JSmall_007_007664.jpg?file_id=d4e3db0da3f5f21b01686b49e3ddce92696592fc</t>
   </si>
@@ -316,13 +319,112 @@
   </si>
   <si>
     <t>Scientific observation station built on Sydney's highest point.</t>
+  </si>
+  <si>
+    <t>Australian Hall</t>
+  </si>
+  <si>
+    <t>Hall located at 150-52 Elizabeth Street used as a club and meeting place by a range of groups, most notably the Aborigines Progressive Association, as a venue for the 1938 Day of Mourning.</t>
+  </si>
+  <si>
+    <t>http://sitesandsounds.net.au/wp-content/uploads/2008/11/australia_hall.jpg</t>
+  </si>
+  <si>
+    <t>https://fbcdn-sphotos-f-a.akamaihd.net/hphotos-ak-prn2/s720x720/253416_416334098415827_2063248121_n.jpg</t>
+  </si>
+  <si>
+    <t>Hotel trading in premises originally built as Sydney Mechanics' School of Arts.</t>
+  </si>
+  <si>
+    <t>Arthouse Hotel</t>
+  </si>
+  <si>
+    <t>Bondi Pavilion</t>
+  </si>
+  <si>
+    <t>Designed to hold 12,000 visitors, the Bondi Pavilion was part of an ambitious improvement scheme for Bondi Beach</t>
+  </si>
+  <si>
+    <t>http://facilities.arts.nsw.gov.au/media/facility_images/Bondi_Pavilion_image_ext.jpg</t>
+  </si>
+  <si>
+    <t>Cadmans Cottage</t>
+  </si>
+  <si>
+    <t>One of the oldest surviving houses in Sydney, built for the government coxswain and his family to live in.</t>
+  </si>
+  <si>
+    <t>http://upload.wikimedia.org/wikipedia/commons/thumb/1/13/Front_of_Cadman%27s_Cottage.jpg/220px-Front_of_Cadman%27s_Cottage.jpg</t>
+  </si>
+  <si>
+    <t>Chifley Tower</t>
+  </si>
+  <si>
+    <t>Modern skyscraper that completes the curve of Chifley Square.</t>
+  </si>
+  <si>
+    <t>http://www.allaboutskyscrapers.com/wp-content/uploads/2012/01/Chifley_Tower_4.jpg</t>
+  </si>
+  <si>
+    <t>Criterion Theatre</t>
+  </si>
+  <si>
+    <t>Theatre behind the Criterion Family Hotel, built in the grand Victorian style which was demolished for road widening.</t>
+  </si>
+  <si>
+    <t>http://www.hat-archive.com/criteriontheatre.jpg</t>
+  </si>
+  <si>
+    <t>Customs House</t>
+  </si>
+  <si>
+    <t>Public building at Circular Quay constructed to house the customs service for the rapidly growing colony. It is now a City of Sydney Library.</t>
+  </si>
+  <si>
+    <t>http://upload.wikimedia.org/wikipedia/commons/0/0b/Customs_House_Sydney.jpg</t>
+  </si>
+  <si>
+    <t>Government House</t>
+  </si>
+  <si>
+    <t>Governor's residence commissioned by Governor Bourke and constructed of local sandstone in the Gothic Revival style.</t>
+  </si>
+  <si>
+    <t>http://www.hht.net.au/__data/assets/image/0014/833/varieties/main_image.jpg</t>
+  </si>
+  <si>
+    <t>Her Majesty's Theatre</t>
+  </si>
+  <si>
+    <t>There have been three Her Majesty's Theatres in Sydney, spanning nearly a century of the city's theatrical history.</t>
+  </si>
+  <si>
+    <t>http://upload.wikimedia.org/wikipedia/commons/5/51/Original_Her_Majesty%27s_Theatre_Sydney.jpg</t>
+  </si>
+  <si>
+    <t>Hero of Waterloo Hotel</t>
+  </si>
+  <si>
+    <t>One of Sydney's oldest hotels, providing refreshment to the changing population of Millers Point</t>
+  </si>
+  <si>
+    <t>http://dictionaryofsydney.org/files/large/9852069fed0afdd2147204fad31a16e3e7788d87</t>
+  </si>
+  <si>
+    <t>Independent Theatre</t>
+  </si>
+  <si>
+    <t>Tram shed, boxing venue, cinema and now theatre</t>
+  </si>
+  <si>
+    <t>http://facilities.arts.nsw.gov.au/media/facility_images/Independent_Theatre_Auditorium_image_int.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,6 +561,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -806,9 +916,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -854,14 +967,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -928,47 +1034,12 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Arab" typeface="Tahoma"/>
+        <a:font script="Hebr" typeface="Gisha"/>
         <a:font script="Thai" typeface="Tahoma"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
@@ -990,7 +1061,42 @@
         <a:font script="Laoo" typeface="DokChampa"/>
         <a:font script="Sinh" typeface="Iskoola Pota"/>
         <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Viet" typeface="Tahoma"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Tahoma"/>
+        <a:font script="Hebr" typeface="Gisha"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Verdana"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
@@ -1145,13 +1251,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40:G44"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="53.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="31.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="53.28515625" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
@@ -1201,7 +1309,7 @@
         <v>-33.925298846270003</v>
       </c>
       <c r="G2" s="1" t="str">
-        <f t="shared" ref="G2:G33" si="0">"insert into Questions (PhotoUrl,Name,Description,Year,Longitude,Latitude,Difficulty) values ('"&amp;A2&amp;"','"&amp;SUBSTITUTE(B2,"'","''")&amp;"','"&amp;SUBSTITUTE(C2,"'","''")&amp;"',"&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;",1)"</f>
+        <f t="shared" ref="G2:G44" si="0">"insert into Questions (PhotoUrl,Name,Description,Year,Longitude,Latitude,Difficulty) values ('"&amp;A2&amp;"','"&amp;SUBSTITUTE(B2,"'","''")&amp;"','"&amp;SUBSTITUTE(C2,"'","''")&amp;"',"&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;",1)"</f>
         <v>insert into Questions (PhotoUrl,Name,Description,Year,Longitude,Latitude,Difficulty) values ('http://dos.heuristscholar.org/heurist/php/fetch_file.php/Liverpool_Arts_H17880.1.jpg?file_id=3ee21ee7de7a98729f56f33ba651a5d6f1b4b8a5','Liverpool Memorial School of Arts hall','Community hall used by the School of Arts but given to Liverpool Council. A painting from the school"s collection was given to the National Gallery in 1963.',1924,150.92292782663,-33.92529884627,1)</v>
       </c>
     </row>
@@ -1528,7 +1636,7 @@
         <v>92</v>
       </c>
       <c r="D16" s="1">
-        <v>1855</v>
+        <v>1906</v>
       </c>
       <c r="E16" s="1">
         <v>151.20651556711999</v>
@@ -1538,7 +1646,7 @@
       </c>
       <c r="G16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Questions (PhotoUrl,Name,Description,Year,Longitude,Latitude,Difficulty) values ('http://dos.heuristscholar.org/heurist/php/fetch_file.php/0803-1022-74.jpg?file_id=cf668f4a5ccf9502beabc4ed7d48330cfaa3dcab','Central Railway Station','Central Railway Station was Sydney''s third terminus, replacing the original 1855 station further north in Redfern and a later upgraded station built in the 1870s.',1855,151.20651556712,-33.882728961646,1)</v>
+        <v>insert into Questions (PhotoUrl,Name,Description,Year,Longitude,Latitude,Difficulty) values ('http://dos.heuristscholar.org/heurist/php/fetch_file.php/0803-1022-74.jpg?file_id=cf668f4a5ccf9502beabc4ed7d48330cfaa3dcab','Central Railway Station','Central Railway Station was Sydney''s third terminus, replacing the original 1855 station further north in Redfern and a later upgraded station built in the 1870s.',1906,151.20651556712,-33.882728961646,1)</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1936,7 +2044,7 @@
         <v>85</v>
       </c>
       <c r="D33" s="1">
-        <v>1986</v>
+        <v>1957</v>
       </c>
       <c r="E33" s="1">
         <v>151.10576477337</v>
@@ -1946,12 +2054,277 @@
       </c>
       <c r="G33" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Questions (PhotoUrl,Name,Description,Year,Longitude,Latitude,Difficulty) values ('http://dos.heuristscholar.org/heurist/php/fetch_file.php/NAA_8890354.jpg?file_id=d4f64e9fa5ac0c02c12a5f21574ec548a5309006','Top Ryde City','Large shopping centre in Ryde, which first opened in 1957, and was redeveloped in 1986 and 2007.',1986,151.10576477337,-33.812665650938,1)</v>
+        <v>insert into Questions (PhotoUrl,Name,Description,Year,Longitude,Latitude,Difficulty) values ('http://dos.heuristscholar.org/heurist/php/fetch_file.php/NAA_8890354.jpg?file_id=d4f64e9fa5ac0c02c12a5f21574ec548a5309006','Top Ryde City','Large shopping centre in Ryde, which first opened in 1957, and was redeveloped in 1986 and 2007.',1957,151.10576477337,-33.812665650938,1)</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1910</v>
+      </c>
+      <c r="E34" s="1">
+        <v>151.209575</v>
+      </c>
+      <c r="F34" s="1">
+        <v>-33.877991999999999</v>
+      </c>
+      <c r="G34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Questions (PhotoUrl,Name,Description,Year,Longitude,Latitude,Difficulty) values ('http://sitesandsounds.net.au/wp-content/uploads/2008/11/australia_hall.jpg','Australian Hall','Hall located at 150-52 Elizabeth Street used as a club and meeting place by a range of groups, most notably the Aborigines Progressive Association, as a venue for the 1938 Day of Mourning.',1910,151.209575,-33.877992,1)</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C35" t="s">
+        <v>103</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1836</v>
+      </c>
+      <c r="E35" s="1">
+        <v>151.20785599999999</v>
+      </c>
+      <c r="F35" s="1">
+        <v>-33.871893999999998</v>
+      </c>
+      <c r="G35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Questions (PhotoUrl,Name,Description,Year,Longitude,Latitude,Difficulty) values ('https://fbcdn-sphotos-f-a.akamaihd.net/hphotos-ak-prn2/s720x720/253416_416334098415827_2063248121_n.jpg','Arthouse Hotel','Hotel trading in premises originally built as Sydney Mechanics'' School of Arts.',1836,151.207856,-33.871894,1)</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1928</v>
+      </c>
+      <c r="E36" s="1">
+        <v>151.27731399999999</v>
+      </c>
+      <c r="F36" s="1">
+        <v>-33.889887000000002</v>
+      </c>
+      <c r="G36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Questions (PhotoUrl,Name,Description,Year,Longitude,Latitude,Difficulty) values ('http://facilities.arts.nsw.gov.au/media/facility_images/Bondi_Pavilion_image_ext.jpg','Bondi Pavilion','Designed to hold 12,000 visitors, the Bondi Pavilion was part of an ambitious improvement scheme for Bondi Beach',1928,151.277314,-33.889887,1)</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" t="s">
+        <v>109</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1815</v>
+      </c>
+      <c r="E37" s="1">
+        <v>151.209113</v>
+      </c>
+      <c r="F37" s="1">
+        <v>-33.858637999999999</v>
+      </c>
+      <c r="G37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Questions (PhotoUrl,Name,Description,Year,Longitude,Latitude,Difficulty) values ('http://upload.wikimedia.org/wikipedia/commons/thumb/1/13/Front_of_Cadman%27s_Cottage.jpg/220px-Front_of_Cadman%27s_Cottage.jpg','Cadmans Cottage','One of the oldest surviving houses in Sydney, built for the government coxswain and his family to live in.',1815,151.209113,-33.858638,1)</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1989</v>
+      </c>
+      <c r="E38" s="1">
+        <v>151.210915</v>
+      </c>
+      <c r="F38" s="1">
+        <v>-33.865979000000003</v>
+      </c>
+      <c r="G38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Questions (PhotoUrl,Name,Description,Year,Longitude,Latitude,Difficulty) values ('http://www.allaboutskyscrapers.com/wp-content/uploads/2012/01/Chifley_Tower_4.jpg','Chifley Tower','Modern skyscraper that completes the curve of Chifley Square.',1989,151.210915,-33.865979,1)</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C39" t="s">
+        <v>115</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1886</v>
+      </c>
+      <c r="E39" s="1">
+        <v>151.20813699999999</v>
+      </c>
+      <c r="F39" s="1">
+        <v>-33.872883000000002</v>
+      </c>
+      <c r="G39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Questions (PhotoUrl,Name,Description,Year,Longitude,Latitude,Difficulty) values ('http://www.hat-archive.com/criteriontheatre.jpg','Criterion Theatre','Theatre behind the Criterion Family Hotel, built in the grand Victorian style which was demolished for road widening.',1886,151.208137,-33.872883,1)</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C40" t="s">
+        <v>118</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1845</v>
+      </c>
+      <c r="E40" s="1">
+        <v>151.21086199999999</v>
+      </c>
+      <c r="F40" s="1">
+        <v>-33.861997000000002</v>
+      </c>
+      <c r="G40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Questions (PhotoUrl,Name,Description,Year,Longitude,Latitude,Difficulty) values ('http://upload.wikimedia.org/wikipedia/commons/0/0b/Customs_House_Sydney.jpg','Customs House','Public building at Circular Quay constructed to house the customs service for the rapidly growing colony. It is now a City of Sydney Library.',1845,151.210862,-33.861997,1)</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C41" t="s">
+        <v>121</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1836</v>
+      </c>
+      <c r="E41" s="1">
+        <v>151.21541999999999</v>
+      </c>
+      <c r="F41" s="1">
+        <v>-33.851028999999997</v>
+      </c>
+      <c r="G41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Questions (PhotoUrl,Name,Description,Year,Longitude,Latitude,Difficulty) values ('http://www.hht.net.au/__data/assets/image/0014/833/varieties/main_image.jpg','Government House','Governor''s residence commissioned by Governor Bourke and constructed of local sandstone in the Gothic Revival style.',1836,151.21542,-33.851029,1)</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C42" t="s">
+        <v>124</v>
+      </c>
+      <c r="D42" s="1">
+        <v>1929</v>
+      </c>
+      <c r="E42" s="1">
+        <v>151.203577</v>
+      </c>
+      <c r="F42" s="1">
+        <v>-33.881985999999998</v>
+      </c>
+      <c r="G42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Questions (PhotoUrl,Name,Description,Year,Longitude,Latitude,Difficulty) values ('http://upload.wikimedia.org/wikipedia/commons/5/51/Original_Her_Majesty%27s_Theatre_Sydney.jpg','Her Majesty''s Theatre','There have been three Her Majesty''s Theatres in Sydney, spanning nearly a century of the city''s theatrical history.',1929,151.203577,-33.881986,1)</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C43" t="s">
+        <v>127</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1844</v>
+      </c>
+      <c r="E43" s="1">
+        <v>151.20593500000001</v>
+      </c>
+      <c r="F43" s="1">
+        <v>-33.856019000000003</v>
+      </c>
+      <c r="G43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Questions (PhotoUrl,Name,Description,Year,Longitude,Latitude,Difficulty) values ('http://dictionaryofsydney.org/files/large/9852069fed0afdd2147204fad31a16e3e7788d87','Hero of Waterloo Hotel','One of Sydney''s oldest hotels, providing refreshment to the changing population of Millers Point',1844,151.205935,-33.856019,1)</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C44" t="s">
+        <v>130</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1911</v>
+      </c>
+      <c r="E44" s="1">
+        <v>151.20809199999999</v>
+      </c>
+      <c r="F44" s="1">
+        <v>-33.832850999999998</v>
+      </c>
+      <c r="G44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Questions (PhotoUrl,Name,Description,Year,Longitude,Latitude,Difficulty) values ('http://facilities.arts.nsw.gov.au/media/facility_images/Independent_Theatre_Auditorium_image_int.jpg','Independent Theatre','Tram shed, boxing venue, cinema and now theatre',1911,151.208092,-33.832851,1)</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G33"/>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1900</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>